<commit_message>
Preço Adicionado na Resposta
</commit_message>
<xml_diff>
--- a/RemédiosPortuguês.xlsx
+++ b/RemédiosPortuguês.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="203">
   <si>
     <t>ID</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Efeitos Colaterais</t>
-  </si>
-  <si>
-    <t>Preço (R$)</t>
   </si>
   <si>
     <t>Abacavir</t>
@@ -1033,1049 +1030,943 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" ht="83.25" customHeight="1">
       <c r="A2" s="4">
         <v>1.0</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="7">
-        <v>10.62</v>
-      </c>
+      <c r="F2" s="7"/>
     </row>
     <row r="3">
       <c r="A3" s="4">
         <v>2.0</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="7">
-        <v>17.84</v>
-      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="4">
         <v>3.0</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="7">
-        <v>19.22</v>
-      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="4">
         <v>4.0</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="7">
-        <v>5.81</v>
-      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="4">
         <v>5.0</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="7">
-        <v>9.74</v>
-      </c>
+      <c r="F6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="4">
         <v>6.0</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="7">
-        <v>21.23</v>
-      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="4">
         <v>7.0</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="7">
-        <v>7.66</v>
-      </c>
+      <c r="F8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="4">
         <v>8.0</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="7">
-        <v>11.54</v>
-      </c>
+      <c r="F9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="4">
         <v>9.0</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="7">
-        <v>5.83</v>
-      </c>
+      <c r="F10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="4">
         <v>10.0</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="7">
-        <v>9.85</v>
-      </c>
+      <c r="F11" s="7"/>
     </row>
     <row r="12">
       <c r="A12" s="4">
         <v>11.0</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="7">
-        <v>9.19</v>
-      </c>
+      <c r="F12" s="7"/>
     </row>
     <row r="13">
       <c r="A13" s="4">
         <v>12.0</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="7">
-        <v>9.11</v>
-      </c>
+      <c r="F13" s="7"/>
     </row>
     <row r="14">
       <c r="A14" s="4">
         <v>13.0</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="7">
-        <v>13.35</v>
-      </c>
+      <c r="F14" s="7"/>
     </row>
     <row r="15">
       <c r="A15" s="4">
         <v>14.0</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="7">
-        <v>17.05</v>
-      </c>
+      <c r="F15" s="7"/>
     </row>
     <row r="16">
       <c r="A16" s="4">
         <v>15.0</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="7">
-        <v>26.94</v>
-      </c>
+      <c r="F16" s="7"/>
     </row>
     <row r="17">
       <c r="A17" s="4">
         <v>16.0</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="7">
-        <v>12.77</v>
-      </c>
+      <c r="F17" s="7"/>
     </row>
     <row r="18">
       <c r="A18" s="4">
         <v>17.0</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="7">
-        <v>27.04</v>
-      </c>
+      <c r="F18" s="7"/>
     </row>
     <row r="19">
       <c r="A19" s="4">
         <v>18.0</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="7">
-        <v>32.11</v>
-      </c>
+      <c r="F19" s="7"/>
     </row>
     <row r="20">
       <c r="A20" s="4">
         <v>19.0</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="7">
-        <v>2963.45</v>
-      </c>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4">
         <v>20.0</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="7">
-        <v>88.89</v>
-      </c>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="4">
         <v>21.0</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="7">
-        <v>15.54</v>
-      </c>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="4">
         <v>22.0</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="7">
-        <v>36.92</v>
-      </c>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="4">
         <v>23.0</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="7">
-        <v>30.81</v>
-      </c>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="4">
         <v>24.0</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="7">
-        <v>4350.0</v>
-      </c>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4">
         <v>25.0</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="7">
-        <v>18.71</v>
-      </c>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="4">
         <v>26.0</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="D27" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F27" s="7">
-        <v>449.0</v>
-      </c>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4">
         <v>27.0</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="D28" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F28" s="7">
-        <v>115.81</v>
-      </c>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="4">
         <v>28.0</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="D29" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="7">
-        <v>14.28</v>
-      </c>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="4">
         <v>29.0</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" s="7">
-        <v>9.0</v>
-      </c>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="4">
         <v>30.0</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="D31" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="13">
-        <v>10.0</v>
-      </c>
+      <c r="F31" s="13"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="4">
         <v>31.0</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="D32" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F32" s="7">
-        <v>211.6</v>
-      </c>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4">
         <v>32.0</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="D33" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F33" s="7">
-        <v>106.98</v>
-      </c>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="4">
         <v>33.0</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="D34" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F34" s="7">
-        <v>3671.98</v>
-      </c>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="4">
         <v>34.0</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="D35" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" s="7">
-        <v>21.12</v>
-      </c>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="4">
         <v>35.0</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="D36" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F36" s="7">
-        <v>14.56</v>
-      </c>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="4">
         <v>36.0</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="D37" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F37" s="7">
-        <v>1100.27</v>
-      </c>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="4">
         <v>37.0</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="D38" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F38" s="7">
-        <v>16.08</v>
-      </c>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="4">
         <v>38.0</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="D39" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F39" s="7">
-        <v>11.54</v>
-      </c>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4">
         <v>39.0</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="D40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F40" s="7">
-        <v>75.36</v>
-      </c>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="4">
         <v>40.0</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F41" s="7">
-        <v>70.25</v>
-      </c>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="4">
         <v>41.0</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="D42" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F42" s="14">
-        <v>8434.77</v>
-      </c>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="4">
         <v>42.0</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="F43" s="7">
-        <v>55.43</v>
-      </c>
+      <c r="F43" s="7"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="4">
         <v>43.0</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F44" s="7">
-        <v>55.51</v>
-      </c>
+      <c r="F44" s="7"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="4">
         <v>44.0</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" s="7">
-        <v>347.93</v>
-      </c>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="4">
         <v>45.0</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="D46" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F46" s="7">
-        <v>14.72</v>
-      </c>
+      <c r="F46" s="7"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="4">
         <v>46.0</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="D47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="F47" s="7">
-        <v>69.39</v>
-      </c>
+      <c r="F47" s="7"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="4">
         <v>47.0</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="D48" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="F48" s="7">
-        <v>120.0</v>
-      </c>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="4">
         <v>48.0</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="D49" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="F49" s="7">
-        <v>11.19</v>
-      </c>
+      <c r="F49" s="7"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="4">
         <v>49.0</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="D50" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="F50" s="7">
-        <v>68.85</v>
-      </c>
+      <c r="F50" s="7"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="4">
         <v>50.0</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>195</v>
-      </c>
       <c r="D51" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F51" s="7">
-        <v>24.21</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="4">
         <v>51.0</v>
       </c>
       <c r="B52" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="F52" s="7">
-        <v>256.47</v>
-      </c>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="4">
         <v>52.0</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="D53" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="E53" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F53" s="7">
-        <v>24.21</v>
-      </c>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1"/>

</xml_diff>